<commit_message>
Change all to combinatory (V2) : everything work fine
</commit_message>
<xml_diff>
--- a/calculMandelbrot.xlsx
+++ b/calculMandelbrot.xlsx
@@ -683,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,10 +709,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>0</v>
+        <v>0.3798828125</v>
       </c>
       <c r="D3" s="1">
-        <v>1</v>
+        <v>0.199951171875</v>
       </c>
       <c r="H3">
         <v>0.38</v>
@@ -747,15 +747,15 @@
       </c>
       <c r="C6" s="1">
         <f>C5^2-D5^2+$C$3</f>
-        <v>0</v>
+        <v>0.3798828125</v>
       </c>
       <c r="D6" s="1">
         <f>2*C5*D5+$D$3</f>
-        <v>1</v>
+        <v>0.199951171875</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" ref="E6:E69" si="0">C6^2+D6^2</f>
-        <v>1</v>
+        <v>0.18429142236709595</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
@@ -764,15 +764,15 @@
       </c>
       <c r="C7" s="1">
         <f t="shared" ref="C7:C30" si="1">C6^2-D6^2+$C$3</f>
-        <v>-1</v>
+        <v>0.48421329259872437</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" ref="D7:D30" si="2">2*C6*D6+$D$3</f>
-        <v>1</v>
+        <v>0.3518671989440918</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0.35827303842205893</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
@@ -781,15 +781,15 @@
       </c>
       <c r="C8" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.49053479953653678</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>0.54070872179141816</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.53299031137765951</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
@@ -798,15 +798,15 @@
       </c>
       <c r="C9" s="1">
         <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>0.32814128023504108</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.73042406077822064</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0.64119600835803747</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
@@ -815,15 +815,15 @@
       </c>
       <c r="C10" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-4.5959796269454012E-2</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>0.67931574471148548</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.46358218388604988</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
@@ -832,15 +832,15 @@
       </c>
       <c r="C11" s="1">
         <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>-7.947476563979039E-2</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.13750874541585539</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>2.5224893439342141E-2</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
@@ -849,15 +849,15 @@
       </c>
       <c r="C12" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.3672903958076571</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>0.17809422124430657</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.16661978649316142</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
@@ -866,15 +866,15 @@
       </c>
       <c r="C13" s="1">
         <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>0.48306749571192942</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.33077576589875562</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0.34276681271930332</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
@@ -883,15 +883,15 @@
       </c>
       <c r="C14" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.50382441060748651</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>0.51952521362481463</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.52374548431589041</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
@@ -900,15 +900,15 @@
       </c>
       <c r="C15" s="1">
         <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>0.36381540163207188</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.72345014097550153</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0.65574175294217873</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
@@ -917,15 +917,15 @@
       </c>
       <c r="C16" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-1.1135647512767244E-2</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>0.72635577907456217</v>
       </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.52771672044054274</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
@@ -934,15 +934,15 @@
       </c>
       <c r="C17" s="1">
         <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>-0.14758590264948557</v>
       </c>
       <c r="D17" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.18377428802572848</v>
       </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>5.5554587600226843E-2</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
@@ -951,15 +951,15 @@
       </c>
       <c r="C18" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.36789142222150001</v>
       </c>
       <c r="D18" s="1">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>0.14570618351091263</v>
       </c>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.15657439045747373</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
@@ -968,15 +968,15 @@
       </c>
       <c r="C19" s="1">
         <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>0.49399661913084225</v>
       </c>
       <c r="D19" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.30715928203159304</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0.33837948425086611</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
@@ -985,15 +985,15 @@
       </c>
       <c r="C20" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.52956864767453871</v>
       </c>
       <c r="D20" s="1">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>0.50342246559152759</v>
       </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.53387713146209248</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
@@ -1002,15 +1002,15 @@
       </c>
       <c r="C21" s="1">
         <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>0.40689158623758692</v>
       </c>
       <c r="D21" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.73314468049957449</v>
       </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0.70306188549576287</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
@@ -1019,15 +1019,15 @@
       </c>
       <c r="C22" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7.9424529061164484E-3</v>
       </c>
       <c r="D22" s="1">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>0.79657197585524142</v>
       </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.63458999527608917</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
@@ -1036,15 +1036,15 @@
       </c>
       <c r="C23" s="1">
         <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>-0.25458101765975738</v>
       </c>
       <c r="D23" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.21260464268412477</v>
       </c>
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0.11001222864352206</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
@@ -1053,15 +1053,15 @@
       </c>
       <c r="C24" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.3994935729618333</v>
       </c>
       <c r="D24" s="1">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>9.1700959287572853E-2</v>
       </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.16800418077207274</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
@@ -1070,15 +1070,15 @@
       </c>
       <c r="C25" s="1">
         <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>0.53106886140355059</v>
       </c>
       <c r="D25" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.27321905961464021</v>
       </c>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0.35668279008917192</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
@@ -1087,15 +1087,15 @@
       </c>
       <c r="C26" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.58726829351575527</v>
       </c>
       <c r="D26" s="1">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>0.49014744168159158</v>
       </c>
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.58512856315591655</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
@@ -1104,15 +1104,15 @@
       </c>
       <c r="C27" s="1">
         <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>0.48452234648189807</v>
       </c>
       <c r="D27" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.77564727516992293</v>
       </c>
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0.83639059971885066</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
@@ -1121,15 +1121,15 @@
       </c>
       <c r="C28" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.301602126179835E-2</v>
       </c>
       <c r="D28" s="1">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>0.95158804749024306</v>
       </c>
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.90568922893578063</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
@@ -1138,15 +1138,15 @@
       </c>
       <c r="C29" s="1">
         <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>-0.5254675828168055</v>
       </c>
       <c r="D29" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.22472295239221235</v>
       </c>
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0.32661658592320891</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
@@ -1155,15 +1155,15 @@
       </c>
       <c r="C30" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.60549858775946386</v>
       </c>
       <c r="D30" s="1">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>-3.6218081318983769E-2</v>
       </c>
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.36794028919313365</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
@@ -1172,15 +1172,15 @@
       </c>
       <c r="C31" s="1">
         <f t="shared" ref="C31:C62" si="3">C30^2-D30^2+$C$3</f>
-        <v>-1</v>
+        <v>0.74519960286427667</v>
       </c>
       <c r="D31" s="1">
         <f t="shared" ref="D31:D62" si="4">2*C30*D30+$D$3</f>
-        <v>1</v>
+        <v>0.15609117769499581</v>
       </c>
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0.57968690386328636</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
@@ -1189,15 +1189,15 @@
       </c>
       <c r="C32" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.91084080485486485</v>
       </c>
       <c r="D32" s="1">
         <f t="shared" si="4"/>
-        <v>-1</v>
+        <v>0.43258933913285624</v>
       </c>
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.0167645081200594</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
@@ -1206,15 +1206,15 @@
       </c>
       <c r="C33" s="1">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>1.0223802479572566</v>
       </c>
       <c r="D33" s="1">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0.98799121552980973</v>
       </c>
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>2.0213880133772122</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
@@ -1223,15 +1223,15 @@
       </c>
       <c r="C34" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.4490175419490704</v>
       </c>
       <c r="D34" s="1">
         <f t="shared" si="4"/>
-        <v>-1</v>
+        <v>2.2201565797009164</v>
       </c>
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>5.1307119913672565</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
@@ -1240,15 +1240,15 @@
       </c>
       <c r="C35" s="1">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>-4.3475956729112859</v>
       </c>
       <c r="D35" s="1">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2.1937296721937218</v>
       </c>
       <c r="E35" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>23.714038009780111</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
@@ -1257,15 +1257,15 @@
       </c>
       <c r="C36" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>14.469021072953765</v>
       </c>
       <c r="D36" s="1">
         <f t="shared" si="4"/>
-        <v>-1</v>
+        <v>-18.874948088858037</v>
       </c>
       <c r="E36" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>565.61623616666589</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
@@ -1274,15 +1274,15 @@
       </c>
       <c r="C37" s="1">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>-146.53121173500557</v>
       </c>
       <c r="D37" s="1">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>-546.00409212531565</v>
       </c>
       <c r="E37" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>319591.86463011923</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
@@ -1291,15 +1291,15 @@
       </c>
       <c r="C38" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-276648.69272224867</v>
       </c>
       <c r="D38" s="1">
         <f t="shared" si="4"/>
-        <v>-1</v>
+        <v>160013.4824139601</v>
       </c>
       <c r="E38" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>102138813739.17189</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
@@ -1308,15 +1308,15 @@
       </c>
       <c r="C39" s="1">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>50930184631.06633</v>
       </c>
       <c r="D39" s="1">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>-88535041455.313232</v>
       </c>
       <c r="E39" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1.0432337272048538E+22</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
@@ -1325,15 +1325,15 @@
       </c>
       <c r="C40" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-5.2445698589395287E+21</v>
       </c>
       <c r="D40" s="1">
         <f t="shared" si="4"/>
-        <v>-1</v>
+        <v>-9.0182120152764284E+21</v>
       </c>
       <c r="E40" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.0883366095777312E+44</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
@@ -1342,15 +1342,15 @@
       </c>
       <c r="C41" s="1">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>-5.3822634947179154E+43</v>
       </c>
       <c r="D41" s="1">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>9.4593285833690123E+43</v>
       </c>
       <c r="E41" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1.184476575747151E+88</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
@@ -1359,15 +1359,15 @@
       </c>
       <c r="C42" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-6.0510136921568899E+87</v>
       </c>
       <c r="D42" s="1">
         <f t="shared" si="4"/>
-        <v>-1</v>
+        <v>-1.0182519783761754E+88</v>
       </c>
       <c r="E42" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.4029847584936966E+176</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
@@ -1376,1069 +1376,1069 @@
       </c>
       <c r="C43" s="1">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>-6.7068942444029363E+175</v>
       </c>
       <c r="D43" s="1">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E43" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1.2322913326440158E+176</v>
+      </c>
+      <c r="E43" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D44" s="1">
-        <f t="shared" si="4"/>
-        <v>-1</v>
-      </c>
-      <c r="E44" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="C44" s="1" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D44" s="1" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E44" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C45" s="1">
-        <f t="shared" si="3"/>
-        <v>-1</v>
-      </c>
-      <c r="D45" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E45" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
+      <c r="C45" s="1" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D45" s="1" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E45" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C46" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D46" s="1">
-        <f t="shared" si="4"/>
-        <v>-1</v>
-      </c>
-      <c r="E46" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="C46" s="1" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D46" s="1" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E46" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C47" s="1">
-        <f t="shared" si="3"/>
-        <v>-1</v>
-      </c>
-      <c r="D47" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E47" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
+      <c r="C47" s="1" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D47" s="1" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E47" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D48" s="1">
-        <f t="shared" si="4"/>
-        <v>-1</v>
-      </c>
-      <c r="E48" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="C48" s="1" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D48" s="1" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E48" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C49" s="1">
-        <f t="shared" si="3"/>
-        <v>-1</v>
-      </c>
-      <c r="D49" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E49" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
+      <c r="C49" s="1" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D49" s="1" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E49" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C50" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D50" s="1">
-        <f t="shared" si="4"/>
-        <v>-1</v>
-      </c>
-      <c r="E50" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="C50" s="1" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D50" s="1" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E50" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C51" s="1">
-        <f t="shared" si="3"/>
-        <v>-1</v>
-      </c>
-      <c r="D51" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E51" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
+      <c r="C51" s="1" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D51" s="1" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E51" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C52" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D52" s="1">
-        <f t="shared" si="4"/>
-        <v>-1</v>
-      </c>
-      <c r="E52" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="C52" s="1" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D52" s="1" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E52" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C53" s="1">
-        <f t="shared" si="3"/>
-        <v>-1</v>
-      </c>
-      <c r="D53" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E53" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
+      <c r="C53" s="1" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D53" s="1" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E53" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C54" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D54" s="1">
-        <f t="shared" si="4"/>
-        <v>-1</v>
-      </c>
-      <c r="E54" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="C54" s="1" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D54" s="1" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E54" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C55" s="1">
-        <f t="shared" si="3"/>
-        <v>-1</v>
-      </c>
-      <c r="D55" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E55" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
+      <c r="C55" s="1" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D55" s="1" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E55" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C56" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D56" s="1">
-        <f t="shared" si="4"/>
-        <v>-1</v>
-      </c>
-      <c r="E56" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="C56" s="1" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D56" s="1" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E56" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C57" s="1">
-        <f t="shared" si="3"/>
-        <v>-1</v>
-      </c>
-      <c r="D57" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E57" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
+      <c r="C57" s="1" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D57" s="1" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E57" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C58" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D58" s="1">
-        <f t="shared" si="4"/>
-        <v>-1</v>
-      </c>
-      <c r="E58" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="C58" s="1" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D58" s="1" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E58" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C59" s="1">
-        <f t="shared" si="3"/>
-        <v>-1</v>
-      </c>
-      <c r="D59" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E59" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
+      <c r="C59" s="1" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D59" s="1" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E59" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C60" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D60" s="1">
-        <f t="shared" si="4"/>
-        <v>-1</v>
-      </c>
-      <c r="E60" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="C60" s="1" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D60" s="1" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E60" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C61" s="1">
-        <f t="shared" si="3"/>
-        <v>-1</v>
-      </c>
-      <c r="D61" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E61" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
+      <c r="C61" s="1" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D61" s="1" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E61" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B62" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C62" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D62" s="1">
-        <f t="shared" si="4"/>
-        <v>-1</v>
-      </c>
-      <c r="E62" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="C62" s="1" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D62" s="1" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E62" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B63" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C63" s="1">
+      <c r="C63" s="1" t="e">
         <f t="shared" ref="C63:C94" si="5">C62^2-D62^2+$C$3</f>
-        <v>-1</v>
-      </c>
-      <c r="D63" s="1">
+        <v>#NUM!</v>
+      </c>
+      <c r="D63" s="1" t="e">
         <f t="shared" ref="D63:D94" si="6">2*C62*D62+$D$3</f>
-        <v>1</v>
-      </c>
-      <c r="E63" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <v>#NUM!</v>
+      </c>
+      <c r="E63" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C64" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="D64" s="1">
-        <f t="shared" si="6"/>
-        <v>-1</v>
-      </c>
-      <c r="E64" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="C64" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D64" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E64" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C65" s="1">
-        <f t="shared" si="5"/>
-        <v>-1</v>
-      </c>
-      <c r="D65" s="1">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="E65" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
+      <c r="C65" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D65" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E65" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C66" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="D66" s="1">
-        <f t="shared" si="6"/>
-        <v>-1</v>
-      </c>
-      <c r="E66" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="C66" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D66" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E66" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C67" s="1">
-        <f t="shared" si="5"/>
-        <v>-1</v>
-      </c>
-      <c r="D67" s="1">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="E67" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
+      <c r="C67" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D67" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E67" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C68" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="D68" s="1">
-        <f t="shared" si="6"/>
-        <v>-1</v>
-      </c>
-      <c r="E68" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="C68" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D68" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E68" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C69" s="1">
-        <f t="shared" si="5"/>
-        <v>-1</v>
-      </c>
-      <c r="D69" s="1">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="E69" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
+      <c r="C69" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D69" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E69" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C70" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="D70" s="1">
-        <f t="shared" si="6"/>
-        <v>-1</v>
-      </c>
-      <c r="E70" s="1">
+      <c r="C70" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D70" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E70" s="1" t="e">
         <f t="shared" ref="E70:E105" si="7">C70^2+D70^2</f>
-        <v>1</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B71" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C71" s="1">
-        <f t="shared" si="5"/>
-        <v>-1</v>
-      </c>
-      <c r="D71" s="1">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="E71" s="1">
-        <f t="shared" si="7"/>
-        <v>2</v>
+      <c r="C71" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D71" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E71" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B72" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C72" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="D72" s="1">
-        <f t="shared" si="6"/>
-        <v>-1</v>
-      </c>
-      <c r="E72" s="1">
-        <f t="shared" si="7"/>
-        <v>1</v>
+      <c r="C72" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D72" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E72" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B73" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C73" s="1">
-        <f t="shared" si="5"/>
-        <v>-1</v>
-      </c>
-      <c r="D73" s="1">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="E73" s="1">
-        <f t="shared" si="7"/>
-        <v>2</v>
+      <c r="C73" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D73" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E73" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C74" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="D74" s="1">
-        <f t="shared" si="6"/>
-        <v>-1</v>
-      </c>
-      <c r="E74" s="1">
-        <f t="shared" si="7"/>
-        <v>1</v>
+      <c r="C74" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D74" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E74" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B75" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C75" s="1">
-        <f t="shared" si="5"/>
-        <v>-1</v>
-      </c>
-      <c r="D75" s="1">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="E75" s="1">
-        <f t="shared" si="7"/>
-        <v>2</v>
+      <c r="C75" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D75" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E75" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C76" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="D76" s="1">
-        <f t="shared" si="6"/>
-        <v>-1</v>
-      </c>
-      <c r="E76" s="1">
-        <f t="shared" si="7"/>
-        <v>1</v>
+      <c r="C76" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D76" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E76" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C77" s="1">
-        <f t="shared" si="5"/>
-        <v>-1</v>
-      </c>
-      <c r="D77" s="1">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="E77" s="1">
-        <f t="shared" si="7"/>
-        <v>2</v>
+      <c r="C77" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D77" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E77" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B78" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C78" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="D78" s="1">
-        <f t="shared" si="6"/>
-        <v>-1</v>
-      </c>
-      <c r="E78" s="1">
-        <f t="shared" si="7"/>
-        <v>1</v>
+      <c r="C78" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D78" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E78" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B79" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C79" s="1">
-        <f t="shared" si="5"/>
-        <v>-1</v>
-      </c>
-      <c r="D79" s="1">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="E79" s="1">
-        <f t="shared" si="7"/>
-        <v>2</v>
+      <c r="C79" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D79" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E79" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B80" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C80" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="D80" s="1">
-        <f t="shared" si="6"/>
-        <v>-1</v>
-      </c>
-      <c r="E80" s="1">
-        <f t="shared" si="7"/>
-        <v>1</v>
+      <c r="C80" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D80" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E80" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B81" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C81" s="1">
-        <f t="shared" si="5"/>
-        <v>-1</v>
-      </c>
-      <c r="D81" s="1">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="E81" s="1">
-        <f t="shared" si="7"/>
-        <v>2</v>
+      <c r="C81" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D81" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E81" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C82" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="D82" s="1">
-        <f t="shared" si="6"/>
-        <v>-1</v>
-      </c>
-      <c r="E82" s="1">
-        <f t="shared" si="7"/>
-        <v>1</v>
+      <c r="C82" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D82" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E82" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B83" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C83" s="1">
-        <f t="shared" si="5"/>
-        <v>-1</v>
-      </c>
-      <c r="D83" s="1">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="E83" s="1">
-        <f t="shared" si="7"/>
-        <v>2</v>
+      <c r="C83" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D83" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E83" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B84" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C84" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="D84" s="1">
-        <f t="shared" si="6"/>
-        <v>-1</v>
-      </c>
-      <c r="E84" s="1">
-        <f t="shared" si="7"/>
-        <v>1</v>
+      <c r="C84" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D84" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E84" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B85" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C85" s="1">
-        <f t="shared" si="5"/>
-        <v>-1</v>
-      </c>
-      <c r="D85" s="1">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="E85" s="1">
-        <f t="shared" si="7"/>
-        <v>2</v>
+      <c r="C85" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D85" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E85" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B86" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C86" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="D86" s="1">
-        <f t="shared" si="6"/>
-        <v>-1</v>
-      </c>
-      <c r="E86" s="1">
-        <f t="shared" si="7"/>
-        <v>1</v>
+      <c r="C86" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D86" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E86" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B87" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C87" s="1">
-        <f t="shared" si="5"/>
-        <v>-1</v>
-      </c>
-      <c r="D87" s="1">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="E87" s="1">
-        <f t="shared" si="7"/>
-        <v>2</v>
+      <c r="C87" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D87" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E87" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B88" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C88" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="D88" s="1">
-        <f t="shared" si="6"/>
-        <v>-1</v>
-      </c>
-      <c r="E88" s="1">
-        <f t="shared" si="7"/>
-        <v>1</v>
+      <c r="C88" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D88" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E88" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B89" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C89" s="1">
-        <f t="shared" si="5"/>
-        <v>-1</v>
-      </c>
-      <c r="D89" s="1">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="E89" s="1">
-        <f t="shared" si="7"/>
-        <v>2</v>
+      <c r="C89" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D89" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E89" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B90" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C90" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="D90" s="1">
-        <f t="shared" si="6"/>
-        <v>-1</v>
-      </c>
-      <c r="E90" s="1">
-        <f t="shared" si="7"/>
-        <v>1</v>
+      <c r="C90" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D90" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E90" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B91" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C91" s="1">
-        <f t="shared" si="5"/>
-        <v>-1</v>
-      </c>
-      <c r="D91" s="1">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="E91" s="1">
-        <f t="shared" si="7"/>
-        <v>2</v>
+      <c r="C91" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D91" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E91" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B92" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C92" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="D92" s="1">
-        <f t="shared" si="6"/>
-        <v>-1</v>
-      </c>
-      <c r="E92" s="1">
-        <f t="shared" si="7"/>
-        <v>1</v>
+      <c r="C92" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D92" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E92" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B93" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C93" s="1">
-        <f t="shared" si="5"/>
-        <v>-1</v>
-      </c>
-      <c r="D93" s="1">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="E93" s="1">
-        <f t="shared" si="7"/>
-        <v>2</v>
+      <c r="C93" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D93" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E93" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B94" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C94" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="D94" s="1">
-        <f t="shared" si="6"/>
-        <v>-1</v>
-      </c>
-      <c r="E94" s="1">
-        <f t="shared" si="7"/>
-        <v>1</v>
+      <c r="C94" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D94" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E94" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B95" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C95" s="1">
+      <c r="C95" s="1" t="e">
         <f t="shared" ref="C95:C105" si="8">C94^2-D94^2+$C$3</f>
-        <v>-1</v>
-      </c>
-      <c r="D95" s="1">
+        <v>#NUM!</v>
+      </c>
+      <c r="D95" s="1" t="e">
         <f t="shared" ref="D95:D105" si="9">2*C94*D94+$D$3</f>
-        <v>1</v>
-      </c>
-      <c r="E95" s="1">
-        <f t="shared" si="7"/>
-        <v>2</v>
+        <v>#NUM!</v>
+      </c>
+      <c r="E95" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B96" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C96" s="1">
+      <c r="C96" s="1" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="D96" s="1">
+        <v>#NUM!</v>
+      </c>
+      <c r="D96" s="1" t="e">
         <f t="shared" si="9"/>
-        <v>-1</v>
-      </c>
-      <c r="E96" s="1">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <v>#NUM!</v>
+      </c>
+      <c r="E96" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B97" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C97" s="1">
+      <c r="C97" s="1" t="e">
         <f t="shared" si="8"/>
-        <v>-1</v>
-      </c>
-      <c r="D97" s="1">
+        <v>#NUM!</v>
+      </c>
+      <c r="D97" s="1" t="e">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="E97" s="1">
-        <f t="shared" si="7"/>
-        <v>2</v>
+        <v>#NUM!</v>
+      </c>
+      <c r="E97" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B98" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C98" s="1">
+      <c r="C98" s="1" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="D98" s="1">
+        <v>#NUM!</v>
+      </c>
+      <c r="D98" s="1" t="e">
         <f t="shared" si="9"/>
-        <v>-1</v>
-      </c>
-      <c r="E98" s="1">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <v>#NUM!</v>
+      </c>
+      <c r="E98" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="99" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B99" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C99" s="1">
+      <c r="C99" s="1" t="e">
         <f t="shared" si="8"/>
-        <v>-1</v>
-      </c>
-      <c r="D99" s="1">
+        <v>#NUM!</v>
+      </c>
+      <c r="D99" s="1" t="e">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="E99" s="1">
-        <f t="shared" si="7"/>
-        <v>2</v>
+        <v>#NUM!</v>
+      </c>
+      <c r="E99" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="100" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B100" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C100" s="1">
+      <c r="C100" s="1" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="D100" s="1">
+        <v>#NUM!</v>
+      </c>
+      <c r="D100" s="1" t="e">
         <f t="shared" si="9"/>
-        <v>-1</v>
-      </c>
-      <c r="E100" s="1">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <v>#NUM!</v>
+      </c>
+      <c r="E100" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="101" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B101" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C101" s="1">
+      <c r="C101" s="1" t="e">
         <f t="shared" si="8"/>
-        <v>-1</v>
-      </c>
-      <c r="D101" s="1">
+        <v>#NUM!</v>
+      </c>
+      <c r="D101" s="1" t="e">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="E101" s="1">
-        <f t="shared" si="7"/>
-        <v>2</v>
+        <v>#NUM!</v>
+      </c>
+      <c r="E101" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="102" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B102" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C102" s="1">
+      <c r="C102" s="1" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="D102" s="1">
+        <v>#NUM!</v>
+      </c>
+      <c r="D102" s="1" t="e">
         <f t="shared" si="9"/>
-        <v>-1</v>
-      </c>
-      <c r="E102" s="1">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <v>#NUM!</v>
+      </c>
+      <c r="E102" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="103" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B103" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C103" s="1">
+      <c r="C103" s="1" t="e">
         <f t="shared" si="8"/>
-        <v>-1</v>
-      </c>
-      <c r="D103" s="1">
+        <v>#NUM!</v>
+      </c>
+      <c r="D103" s="1" t="e">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="E103" s="1">
-        <f t="shared" si="7"/>
-        <v>2</v>
+        <v>#NUM!</v>
+      </c>
+      <c r="E103" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="104" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B104" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C104" s="1">
+      <c r="C104" s="1" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="D104" s="1">
+        <v>#NUM!</v>
+      </c>
+      <c r="D104" s="1" t="e">
         <f t="shared" si="9"/>
-        <v>-1</v>
-      </c>
-      <c r="E104" s="1">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <v>#NUM!</v>
+      </c>
+      <c r="E104" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="105" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B105" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C105" s="1">
+      <c r="C105" s="1" t="e">
         <f t="shared" si="8"/>
-        <v>-1</v>
-      </c>
-      <c r="D105" s="1">
+        <v>#NUM!</v>
+      </c>
+      <c r="D105" s="1" t="e">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="E105" s="1">
-        <f t="shared" si="7"/>
-        <v>2</v>
+        <v>#NUM!</v>
+      </c>
+      <c r="E105" s="1" t="e">
+        <f t="shared" si="7"/>
+        <v>#NUM!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>